<commit_message>
Vehicles now need services, some fixes
</commit_message>
<xml_diff>
--- a/simulation.xlsx
+++ b/simulation.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\SovietRepublic\media_soviet\workshop_wip\2950484463\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A67208F0-EAA4-49BC-B5D1-3B7C1B4E657A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84934FB4-E96C-4510-8F80-D7A7D2534167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{37B42EF0-A527-4E43-8B50-C599F805ECB4}"/>
   </bookViews>
@@ -20,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>population</t>
   </si>
@@ -66,9 +55,6 @@
   </si>
   <si>
     <t>monthly balance</t>
-  </si>
-  <si>
-    <t>INTERNAL_DEMAND_FACTOR</t>
   </si>
   <si>
     <t>PRICE_BUY_RUB</t>
@@ -427,15 +413,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F174D880-89ED-4B1D-B390-99E3C5AB2516}">
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -472,16 +458,13 @@
       <c r="N1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>20000</v>
       </c>
       <c r="B2">
-        <f>A2*$M$2</f>
+        <f>800</f>
         <v>800</v>
       </c>
       <c r="C2">
@@ -500,7 +483,7 @@
         <v>2</v>
       </c>
       <c r="G2">
-        <f>D2*F2*IF(D2&lt;0,$N$2,$O$2)</f>
+        <f>D2*F2*IF(D2&lt;0,$M$2,$N$2)</f>
         <v>-9600</v>
       </c>
       <c r="H2">
@@ -514,268 +497,265 @@
         <v>0.03</v>
       </c>
       <c r="M2">
-        <v>0.04</v>
+        <v>6</v>
       </c>
       <c r="N2">
-        <v>6</v>
-      </c>
-      <c r="O2">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>20000</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B10" si="0">A3*$M$2</f>
+        <f>800</f>
         <v>800</v>
       </c>
       <c r="C3">
         <v>200</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D8" si="1">C3-B3</f>
+        <f t="shared" ref="D3:D8" si="0">C3-B3</f>
         <v>-600</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E10" si="2">$K$2+$L$2*A3+C3</f>
+        <f t="shared" ref="E3:E10" si="1">$K$2+$L$2*A3+C3</f>
         <v>1000</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F10" si="3">1-D3/E3</f>
+        <f t="shared" ref="F3:F10" si="2">1-D3/E3</f>
         <v>1.6</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G10" si="4">D3*F3*IF(D3&lt;0,$N$2,$O$2)</f>
+        <f t="shared" ref="G3:G10" si="3">D3*F3*IF(D3&lt;0,$M$2,$N$2)</f>
         <v>-5760</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H10" si="5">G3*30</f>
+        <f t="shared" ref="H3:H10" si="4">G3*30</f>
         <v>-172800</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>20000</v>
       </c>
       <c r="B4">
-        <f t="shared" si="0"/>
+        <f>800</f>
         <v>800</v>
       </c>
       <c r="C4">
         <v>400</v>
       </c>
       <c r="D4">
+        <f t="shared" si="0"/>
+        <v>-400</v>
+      </c>
+      <c r="E4">
         <f t="shared" si="1"/>
-        <v>-400</v>
-      </c>
-      <c r="E4">
+        <v>1200</v>
+      </c>
+      <c r="F4">
         <f t="shared" si="2"/>
-        <v>1200</v>
-      </c>
-      <c r="F4">
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="G4">
         <f t="shared" si="3"/>
-        <v>1.3333333333333333</v>
-      </c>
-      <c r="G4">
+        <v>-3199.9999999999995</v>
+      </c>
+      <c r="H4">
         <f t="shared" si="4"/>
-        <v>-3199.9999999999995</v>
-      </c>
-      <c r="H4">
-        <f t="shared" si="5"/>
         <v>-95999.999999999985</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>20000</v>
       </c>
       <c r="B5">
-        <f t="shared" si="0"/>
+        <f>800</f>
         <v>800</v>
       </c>
       <c r="C5">
         <v>600</v>
       </c>
       <c r="D5">
+        <f t="shared" si="0"/>
+        <v>-200</v>
+      </c>
+      <c r="E5">
         <f t="shared" si="1"/>
-        <v>-200</v>
-      </c>
-      <c r="E5">
+        <v>1400</v>
+      </c>
+      <c r="F5">
         <f t="shared" si="2"/>
-        <v>1400</v>
-      </c>
-      <c r="F5">
+        <v>1.1428571428571428</v>
+      </c>
+      <c r="G5">
         <f t="shared" si="3"/>
-        <v>1.1428571428571428</v>
-      </c>
-      <c r="G5">
+        <v>-1371.4285714285713</v>
+      </c>
+      <c r="H5">
         <f t="shared" si="4"/>
-        <v>-1371.4285714285713</v>
-      </c>
-      <c r="H5">
-        <f t="shared" si="5"/>
         <v>-41142.857142857138</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>20000</v>
       </c>
       <c r="B6">
+        <f>800</f>
+        <v>800</v>
+      </c>
+      <c r="C6">
+        <v>800</v>
+      </c>
+      <c r="D6">
         <f t="shared" si="0"/>
-        <v>800</v>
-      </c>
-      <c r="C6">
-        <v>800</v>
-      </c>
-      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
         <f t="shared" si="1"/>
+        <v>1600</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E6">
-        <f t="shared" si="2"/>
-        <v>1600</v>
-      </c>
-      <c r="F6">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="G6">
+      <c r="H6">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="H6">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>20000</v>
       </c>
       <c r="B7">
-        <f t="shared" si="0"/>
+        <f>800</f>
         <v>800</v>
       </c>
       <c r="C7">
         <v>1000</v>
       </c>
       <c r="D7">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="E7">
         <f t="shared" si="1"/>
-        <v>200</v>
-      </c>
-      <c r="E7">
+        <v>1800</v>
+      </c>
+      <c r="F7">
         <f t="shared" si="2"/>
-        <v>1800</v>
-      </c>
-      <c r="F7">
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="G7">
         <f t="shared" si="3"/>
-        <v>0.88888888888888884</v>
-      </c>
-      <c r="G7">
+        <v>888.88888888888891</v>
+      </c>
+      <c r="H7">
         <f t="shared" si="4"/>
-        <v>888.88888888888891</v>
-      </c>
-      <c r="H7">
-        <f t="shared" si="5"/>
         <v>26666.666666666668</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>20000</v>
       </c>
       <c r="B8">
-        <f t="shared" si="0"/>
+        <f>800</f>
         <v>800</v>
       </c>
       <c r="C8">
         <v>1200</v>
       </c>
       <c r="D8">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+      <c r="E8">
         <f t="shared" si="1"/>
-        <v>400</v>
-      </c>
-      <c r="E8">
+        <v>2000</v>
+      </c>
+      <c r="F8">
         <f t="shared" si="2"/>
-        <v>2000</v>
-      </c>
-      <c r="F8">
+        <v>0.8</v>
+      </c>
+      <c r="G8">
         <f t="shared" si="3"/>
-        <v>0.8</v>
-      </c>
-      <c r="G8">
+        <v>1600</v>
+      </c>
+      <c r="H8">
         <f t="shared" si="4"/>
-        <v>1600</v>
-      </c>
-      <c r="H8">
-        <f t="shared" si="5"/>
         <v>48000</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>20000</v>
       </c>
       <c r="B9">
-        <f t="shared" si="0"/>
+        <f>800</f>
         <v>800</v>
       </c>
       <c r="C9">
         <v>1400</v>
       </c>
       <c r="D9">
-        <f t="shared" ref="D9:D10" si="6">C9-B9</f>
+        <f t="shared" ref="D9:D10" si="5">C9-B9</f>
         <v>600</v>
       </c>
       <c r="E9">
+        <f t="shared" si="1"/>
+        <v>2200</v>
+      </c>
+      <c r="F9">
         <f t="shared" si="2"/>
-        <v>2200</v>
-      </c>
-      <c r="F9">
+        <v>0.72727272727272729</v>
+      </c>
+      <c r="G9">
         <f t="shared" si="3"/>
-        <v>0.72727272727272729</v>
-      </c>
-      <c r="G9">
+        <v>2181.818181818182</v>
+      </c>
+      <c r="H9">
         <f t="shared" si="4"/>
-        <v>2181.818181818182</v>
-      </c>
-      <c r="H9">
-        <f t="shared" si="5"/>
         <v>65454.545454545456</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>20000</v>
       </c>
       <c r="B10">
-        <f t="shared" si="0"/>
+        <f>800</f>
         <v>800</v>
       </c>
       <c r="C10">
         <v>1600</v>
       </c>
       <c r="D10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>800</v>
       </c>
       <c r="E10">
+        <f t="shared" si="1"/>
+        <v>2400</v>
+      </c>
+      <c r="F10">
         <f t="shared" si="2"/>
-        <v>2400</v>
-      </c>
-      <c r="F10">
+        <v>0.66666666666666674</v>
+      </c>
+      <c r="G10">
         <f t="shared" si="3"/>
-        <v>0.66666666666666674</v>
-      </c>
-      <c r="G10">
+        <v>2666.666666666667</v>
+      </c>
+      <c r="H10">
         <f t="shared" si="4"/>
-        <v>2666.666666666667</v>
-      </c>
-      <c r="H10">
-        <f t="shared" si="5"/>
         <v>80000.000000000015</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Balance, objectives toggle, critical section
</commit_message>
<xml_diff>
--- a/simulation.xlsx
+++ b/simulation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Steam\steamapps\common\SovietRepublic\media_soviet\workshop_wip\2950484463\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A67208F0-EAA4-49BC-B5D1-3B7C1B4E657A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{175AB820-9860-4EBA-AC6E-38D5EA9B13F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{37B42EF0-A527-4E43-8B50-C599F805ECB4}"/>
   </bookViews>
@@ -19,17 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -430,7 +419,7 @@
   <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,14 +471,14 @@
       </c>
       <c r="B2">
         <f>A2*$M$2</f>
-        <v>800</v>
+        <v>400</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
         <f>C2-B2</f>
-        <v>-800</v>
+        <v>-400</v>
       </c>
       <c r="E2">
         <f>$K$2+$L$2*A2</f>
@@ -497,15 +486,15 @@
       </c>
       <c r="F2">
         <f>1-D2/E2</f>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="G2">
         <f>D2*F2*IF(D2&lt;0,$N$2,$O$2)</f>
-        <v>-9600</v>
+        <v>-3600</v>
       </c>
       <c r="H2">
         <f>G2*30</f>
-        <v>-288000</v>
+        <v>-108000</v>
       </c>
       <c r="K2">
         <v>200</v>
@@ -514,7 +503,7 @@
         <v>0.03</v>
       </c>
       <c r="M2">
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
       <c r="N2">
         <v>6</v>
@@ -529,14 +518,14 @@
       </c>
       <c r="B3">
         <f t="shared" ref="B3:B10" si="0">A3*$M$2</f>
-        <v>800</v>
+        <v>400</v>
       </c>
       <c r="C3">
         <v>200</v>
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D8" si="1">C3-B3</f>
-        <v>-600</v>
+        <v>-200</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E10" si="2">$K$2+$L$2*A3+C3</f>
@@ -544,15 +533,15 @@
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F10" si="3">1-D3/E3</f>
-        <v>1.6</v>
+        <v>1.2</v>
       </c>
       <c r="G3">
         <f t="shared" ref="G3:G10" si="4">D3*F3*IF(D3&lt;0,$N$2,$O$2)</f>
-        <v>-5760</v>
+        <v>-1440</v>
       </c>
       <c r="H3">
         <f t="shared" ref="H3:H10" si="5">G3*30</f>
-        <v>-172800</v>
+        <v>-43200</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -561,14 +550,14 @@
       </c>
       <c r="B4">
         <f t="shared" si="0"/>
-        <v>800</v>
+        <v>400</v>
       </c>
       <c r="C4">
         <v>400</v>
       </c>
       <c r="D4">
         <f t="shared" si="1"/>
-        <v>-400</v>
+        <v>0</v>
       </c>
       <c r="E4">
         <f t="shared" si="2"/>
@@ -576,15 +565,15 @@
       </c>
       <c r="F4">
         <f t="shared" si="3"/>
-        <v>1.3333333333333333</v>
+        <v>1</v>
       </c>
       <c r="G4">
         <f t="shared" si="4"/>
-        <v>-3199.9999999999995</v>
+        <v>0</v>
       </c>
       <c r="H4">
         <f t="shared" si="5"/>
-        <v>-95999.999999999985</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -593,14 +582,14 @@
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
-        <v>800</v>
+        <v>400</v>
       </c>
       <c r="C5">
         <v>600</v>
       </c>
       <c r="D5">
         <f t="shared" si="1"/>
-        <v>-200</v>
+        <v>200</v>
       </c>
       <c r="E5">
         <f t="shared" si="2"/>
@@ -608,15 +597,15 @@
       </c>
       <c r="F5">
         <f t="shared" si="3"/>
-        <v>1.1428571428571428</v>
+        <v>0.85714285714285721</v>
       </c>
       <c r="G5">
         <f t="shared" si="4"/>
-        <v>-1371.4285714285713</v>
+        <v>857.14285714285722</v>
       </c>
       <c r="H5">
         <f t="shared" si="5"/>
-        <v>-41142.857142857138</v>
+        <v>25714.285714285717</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -625,14 +614,14 @@
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
-        <v>800</v>
+        <v>400</v>
       </c>
       <c r="C6">
         <v>800</v>
       </c>
       <c r="D6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="E6">
         <f t="shared" si="2"/>
@@ -640,15 +629,15 @@
       </c>
       <c r="F6">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="G6">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1500</v>
       </c>
       <c r="H6">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>45000</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -657,14 +646,14 @@
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
-        <v>800</v>
+        <v>400</v>
       </c>
       <c r="C7">
         <v>1000</v>
       </c>
       <c r="D7">
         <f t="shared" si="1"/>
-        <v>200</v>
+        <v>600</v>
       </c>
       <c r="E7">
         <f t="shared" si="2"/>
@@ -672,15 +661,15 @@
       </c>
       <c r="F7">
         <f t="shared" si="3"/>
-        <v>0.88888888888888884</v>
+        <v>0.66666666666666674</v>
       </c>
       <c r="G7">
         <f t="shared" si="4"/>
-        <v>888.88888888888891</v>
+        <v>2000.0000000000002</v>
       </c>
       <c r="H7">
         <f t="shared" si="5"/>
-        <v>26666.666666666668</v>
+        <v>60000.000000000007</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -689,14 +678,14 @@
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
-        <v>800</v>
+        <v>400</v>
       </c>
       <c r="C8">
         <v>1200</v>
       </c>
       <c r="D8">
         <f t="shared" si="1"/>
-        <v>400</v>
+        <v>800</v>
       </c>
       <c r="E8">
         <f t="shared" si="2"/>
@@ -704,15 +693,15 @@
       </c>
       <c r="F8">
         <f t="shared" si="3"/>
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="G8">
         <f t="shared" si="4"/>
-        <v>1600</v>
+        <v>2400</v>
       </c>
       <c r="H8">
         <f t="shared" si="5"/>
-        <v>48000</v>
+        <v>72000</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -721,14 +710,14 @@
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
-        <v>800</v>
+        <v>400</v>
       </c>
       <c r="C9">
         <v>1400</v>
       </c>
       <c r="D9">
         <f t="shared" ref="D9:D10" si="6">C9-B9</f>
-        <v>600</v>
+        <v>1000</v>
       </c>
       <c r="E9">
         <f t="shared" si="2"/>
@@ -736,15 +725,15 @@
       </c>
       <c r="F9">
         <f t="shared" si="3"/>
-        <v>0.72727272727272729</v>
+        <v>0.54545454545454541</v>
       </c>
       <c r="G9">
         <f t="shared" si="4"/>
-        <v>2181.818181818182</v>
+        <v>2727.272727272727</v>
       </c>
       <c r="H9">
         <f t="shared" si="5"/>
-        <v>65454.545454545456</v>
+        <v>81818.181818181809</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -753,14 +742,14 @@
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
-        <v>800</v>
+        <v>400</v>
       </c>
       <c r="C10">
         <v>1600</v>
       </c>
       <c r="D10">
         <f t="shared" si="6"/>
-        <v>800</v>
+        <v>1200</v>
       </c>
       <c r="E10">
         <f t="shared" si="2"/>
@@ -768,15 +757,15 @@
       </c>
       <c r="F10">
         <f t="shared" si="3"/>
-        <v>0.66666666666666674</v>
+        <v>0.5</v>
       </c>
       <c r="G10">
         <f t="shared" si="4"/>
-        <v>2666.666666666667</v>
+        <v>3000</v>
       </c>
       <c r="H10">
         <f t="shared" si="5"/>
-        <v>80000.000000000015</v>
+        <v>90000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>